<commit_message>
add separator and remove unused stuff
</commit_message>
<xml_diff>
--- a/CoUML-app/ClientApp/src/assets/consts.xlsx
+++ b/CoUML-app/ClientApp/src/assets/consts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smurph/Documents/CoUML/CoUML/CoUML-app/ClientApp/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B2843C-32BF-6345-880D-FBAE31FF72AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5205E78-8C98-7945-8FF5-17FAA65C46DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21520" yWindow="6820" windowWidth="21600" windowHeight="18920" xr2:uid="{2D55D91E-6242-7C43-A416-06FB51B3D50D}"/>
   </bookViews>
@@ -1151,8 +1151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338AB3BC-E281-BB41-9996-004E373358F6}">
   <dimension ref="D10:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>